<commit_message>
student details on navbar make pending category more accurate
</commit_message>
<xml_diff>
--- a/admin/uploads/Question With Images.xlsx
+++ b/admin/uploads/Question With Images.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\admin\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246A54FE-8AC9-4B20-A8D9-8EFD2313965B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C40BD57-53A0-4865-A69B-B2A87F9ECE0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1485,7 +1485,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1786,7 +1786,7 @@
         <v>36</v>
       </c>
       <c r="B8" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="5">
         <v>1</v>

</xml_diff>